<commit_message>
FIX TIMEDATE & CREATE ROOM(block same name)
</commit_message>
<xml_diff>
--- a/LT_DB.xlsx
+++ b/LT_DB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>user_idx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -435,6 +435,30 @@
       </rPr>
       <t>group_create_check.php</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공적으로 생성됨 알림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>실패 알림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME_FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 해당 방 이름이 존재</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -838,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -853,7 +877,7 @@
     <col min="7" max="7" width="13.375" customWidth="1"/>
     <col min="8" max="8" width="15.125" customWidth="1"/>
     <col min="9" max="9" width="14.75" customWidth="1"/>
-    <col min="10" max="10" width="19.375" customWidth="1"/>
+    <col min="10" max="10" width="21.375" customWidth="1"/>
     <col min="11" max="11" width="19.875" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
     <col min="13" max="13" width="17.125" customWidth="1"/>
@@ -1105,7 +1129,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -1122,12 +1146,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>69</v>
       </c>
@@ -1141,16 +1165,28 @@
       <c r="G43" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>97</v>
+      </c>
+      <c r="J43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
         <v>70</v>
       </c>
       <c r="G44" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
         <v>72</v>
       </c>
@@ -1158,12 +1194,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>76</v>
       </c>
@@ -1177,16 +1213,28 @@
       <c r="G47" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F48" t="s">
         <v>70</v>
       </c>
       <c r="G48" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>99</v>
+      </c>
+      <c r="J48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
         <v>72</v>
       </c>
@@ -1194,12 +1242,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>96</v>
       </c>
@@ -1213,24 +1261,42 @@
       <c r="G51" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>97</v>
+      </c>
+      <c r="J51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
         <v>83</v>
       </c>
       <c r="G52" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>99</v>
+      </c>
+      <c r="J52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F53" t="s">
         <v>84</v>
       </c>
       <c r="G53" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>101</v>
+      </c>
+      <c r="J53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
         <v>85</v>
       </c>
@@ -1238,7 +1304,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F55" t="s">
         <v>86</v>
       </c>
@@ -1246,7 +1312,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>87</v>
       </c>
@@ -1254,7 +1320,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F57" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Division sheet & add user_create_check.php
</commit_message>
<xml_diff>
--- a/LT_DB.xlsx
+++ b/LT_DB.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="12465"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="php" sheetId="1" r:id="rId1"/>
+    <sheet name="Database" sheetId="3" r:id="rId2"/>
+    <sheet name="Level exp" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t>user_idx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -58,18 +60,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>user_friends</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_games</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_achievenemt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>user_exp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -121,18 +111,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>01AB23CE,01AB23CF,01AB23CG,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>AB01CD23</t>
-  </si>
-  <si>
-    <t>AB01CD23</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A0B1C2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -300,10 +279,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>http://lemontree.dothome.co.kr/pinbox/bbs_write_check.php</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>content</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -328,23 +303,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>http://lemontree.dothome.co.kr/pinbox/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>comment_write_check.php</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>글 쓰기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -421,23 +379,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>http://lemontree.dothome.co.kr/pinbox/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>group_create_check.php</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SUCCESS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -459,6 +400,118 @@
   </si>
   <si>
     <t>이미 해당 방 이름이 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_pw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_sex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_age</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_phone</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_profile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성별 (false:남자 | true:여자)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전화번호 ('-'기호 없이 ex 01012345678)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로필 사진 (사진 이름이 text로 들어옴)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/bbs/bbs_write_check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/comment/comment_write_check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/group/group_create_check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/user/user_create_check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID_FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 해당 ID가 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 해당 이름이 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMAIL_FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 해당 이메일이 존재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHONE_FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 해당 전화번호가 존재</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +519,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,8 +561,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -558,24 +628,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -860,10 +948,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O57"/>
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -885,461 +976,695 @@
     <col min="15" max="15" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2">
-        <v>54321</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L25" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="G8" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" t="s">
+      <c r="G13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
         <v>79</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
         <v>80</v>
       </c>
-      <c r="I43" t="s">
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
         <v>97</v>
       </c>
-      <c r="J43" t="s">
+      <c r="G19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F44" t="s">
-        <v>70</v>
-      </c>
-      <c r="G44" t="s">
-        <v>71</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="J19" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
         <v>99</v>
       </c>
-      <c r="J44" t="s">
+      <c r="G20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F45" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" t="s">
-        <v>74</v>
-      </c>
-      <c r="G47" t="s">
-        <v>75</v>
-      </c>
-      <c r="I47" t="s">
-        <v>97</v>
-      </c>
-      <c r="J47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F48" t="s">
-        <v>70</v>
-      </c>
-      <c r="G48" t="s">
-        <v>71</v>
-      </c>
-      <c r="I48" t="s">
-        <v>99</v>
-      </c>
-      <c r="J48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F49" t="s">
-        <v>72</v>
-      </c>
-      <c r="G49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" t="s">
-        <v>82</v>
-      </c>
-      <c r="G51" t="s">
-        <v>89</v>
-      </c>
-      <c r="I51" t="s">
-        <v>97</v>
-      </c>
-      <c r="J51" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F52" t="s">
-        <v>83</v>
-      </c>
-      <c r="G52" t="s">
-        <v>90</v>
-      </c>
-      <c r="I52" t="s">
-        <v>99</v>
-      </c>
-      <c r="J52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F53" t="s">
-        <v>84</v>
-      </c>
-      <c r="G53" t="s">
-        <v>91</v>
-      </c>
-      <c r="I53" t="s">
+      <c r="J20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
         <v>101</v>
       </c>
-      <c r="J53" t="s">
+      <c r="G21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F54" t="s">
-        <v>85</v>
-      </c>
-      <c r="G54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F55" t="s">
-        <v>86</v>
-      </c>
-      <c r="G55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F56" t="s">
-        <v>87</v>
-      </c>
-      <c r="G56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F57" t="s">
-        <v>88</v>
-      </c>
-      <c r="G57" t="s">
-        <v>95</v>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" t="s">
+        <v>120</v>
+      </c>
+      <c r="K23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A51:E51"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1"/>
-    <hyperlink ref="A43" r:id="rId2"/>
+    <hyperlink ref="A18" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="A10" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:M36"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="14.375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="23.75" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="16" style="7" customWidth="1"/>
+    <col min="11" max="11" width="18.625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="7" customWidth="1"/>
+    <col min="13" max="13" width="14.875" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8">
+        <v>20</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="8">
+        <v>54321</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="C1">
+        <v>200</v>
+      </c>
+      <c r="D1">
+        <v>300</v>
+      </c>
+      <c r="E1">
+        <v>500</v>
+      </c>
+      <c r="F1">
+        <v>800</v>
+      </c>
+      <c r="G1">
+        <v>1300</v>
+      </c>
+      <c r="H1">
+        <v>2100</v>
+      </c>
+      <c r="I1">
+        <v>3400</v>
+      </c>
+      <c r="J1">
+        <v>5500</v>
+      </c>
+      <c r="K1">
+        <v>8900</v>
+      </c>
+      <c r="L1">
+        <v>14400</v>
+      </c>
+      <c r="M1">
+        <v>23300</v>
+      </c>
+      <c r="N1">
+        <v>37700</v>
+      </c>
+      <c r="O1">
+        <v>61000</v>
+      </c>
+      <c r="P1">
+        <v>98700</v>
+      </c>
+      <c r="Q1">
+        <v>159700</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add follow/unfollow/following & bring comment
</commit_message>
<xml_diff>
--- a/LT_DB.xlsx
+++ b/LT_DB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="184">
   <si>
     <t>user_idx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -681,6 +681,86 @@
   </si>
   <si>
     <t>PB_BBS 테이블 확인할 것</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 팔로우</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>target_token</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>타겟 유저 토큰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공적으로 팔로우 함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALREADY_FOLLOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 팔로우 했음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 가져오기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/comment/comment_bring</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>글 인덱스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>json(댓글정보)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB_COMMENT 테이븍 확인할 것</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/user/user_follow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔로우 중인지 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/user/user_is_following</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UN_FOLLOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔로우 안되어 있음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 언 팔로우</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/user/user_unfollow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALREADY_UNFOLLOW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 언 팔로우 했음</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1129,10 +1209,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1694,8 +1774,182 @@
         <v>161</v>
       </c>
     </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>149</v>
+      </c>
+      <c r="J49" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" t="s">
+        <v>166</v>
+      </c>
+      <c r="J50" t="s">
+        <v>78</v>
+      </c>
+      <c r="K50" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>168</v>
+      </c>
+      <c r="K51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" t="s">
+        <v>173</v>
+      </c>
+      <c r="K54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J55" t="s">
+        <v>78</v>
+      </c>
+      <c r="K55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>149</v>
+      </c>
+      <c r="J58" t="s">
+        <v>168</v>
+      </c>
+      <c r="K58" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>165</v>
+      </c>
+      <c r="G59" t="s">
+        <v>166</v>
+      </c>
+      <c r="J59" t="s">
+        <v>78</v>
+      </c>
+      <c r="K59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J60" t="s">
+        <v>178</v>
+      </c>
+      <c r="K60" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>149</v>
+      </c>
+      <c r="J63" t="s">
+        <v>182</v>
+      </c>
+      <c r="K63" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>165</v>
+      </c>
+      <c r="G64" t="s">
+        <v>166</v>
+      </c>
+      <c r="J64" t="s">
+        <v>78</v>
+      </c>
+      <c r="K64" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A63:E63"/>
     <mergeCell ref="A44:E44"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A36:E36"/>
@@ -1717,9 +1971,13 @@
     <hyperlink ref="A36" r:id="rId7"/>
     <hyperlink ref="A40" r:id="rId8"/>
     <hyperlink ref="A44" r:id="rId9"/>
+    <hyperlink ref="A49" r:id="rId10"/>
+    <hyperlink ref="A54" r:id="rId11"/>
+    <hyperlink ref="A58" r:id="rId12"/>
+    <hyperlink ref="A63" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add unjoin_room & fix join_room
</commit_message>
<xml_diff>
--- a/LT_DB.xlsx
+++ b/LT_DB.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="191">
   <si>
     <t>user_idx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -761,6 +761,34 @@
   </si>
   <si>
     <t>이미 언 팔로우 했음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>방탈퇴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lemontree.dothome.co.kr/pinbox/room/room_unjoin_check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공적으로 탈퇴됨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT_FOUND_ROOM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘못된 방 입력</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT_FOUND_ROOM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘못된 방 입력</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1211,8 +1239,8 @@
   </sheetPr>
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1678,52 +1706,60 @@
         <v>127</v>
       </c>
     </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>146</v>
+      <c r="A39" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J39" t="s">
+        <v>76</v>
+      </c>
+      <c r="K39" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
       <c r="F40" t="s">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="G40" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="J40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K40" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F41" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" t="s">
-        <v>139</v>
-      </c>
       <c r="J41" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="K41" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J42" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="K42" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -1774,184 +1810,228 @@
         <v>161</v>
       </c>
     </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>164</v>
+      <c r="A48" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>149</v>
+      </c>
+      <c r="J48" t="s">
+        <v>76</v>
+      </c>
+      <c r="K48" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
       <c r="F49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" t="s">
+        <v>166</v>
+      </c>
+      <c r="J49" t="s">
+        <v>78</v>
+      </c>
+      <c r="K49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>168</v>
+      </c>
+      <c r="K50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" t="s">
+        <v>172</v>
+      </c>
+      <c r="J52" t="s">
+        <v>173</v>
+      </c>
+      <c r="K52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J53" t="s">
+        <v>78</v>
+      </c>
+      <c r="K53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" t="s">
         <v>1</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G55" t="s">
         <v>149</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J55" t="s">
+        <v>168</v>
+      </c>
+      <c r="K55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>165</v>
+      </c>
+      <c r="G56" t="s">
+        <v>166</v>
+      </c>
+      <c r="J56" t="s">
+        <v>78</v>
+      </c>
+      <c r="K56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J57" t="s">
+        <v>178</v>
+      </c>
+      <c r="K57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" t="s">
+        <v>1</v>
+      </c>
+      <c r="G59" t="s">
+        <v>149</v>
+      </c>
+      <c r="J59" t="s">
+        <v>182</v>
+      </c>
+      <c r="K59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>165</v>
+      </c>
+      <c r="G60" t="s">
+        <v>166</v>
+      </c>
+      <c r="J60" t="s">
+        <v>78</v>
+      </c>
+      <c r="K60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>184</v>
+      </c>
+      <c r="J61" t="s">
         <v>76</v>
       </c>
-      <c r="K49" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F50" t="s">
-        <v>165</v>
-      </c>
-      <c r="G50" t="s">
-        <v>166</v>
-      </c>
-      <c r="J50" t="s">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>149</v>
+      </c>
+      <c r="J62" t="s">
         <v>78</v>
       </c>
-      <c r="K50" t="s">
+      <c r="K62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>45</v>
+      </c>
+      <c r="G63" t="s">
+        <v>139</v>
+      </c>
+      <c r="J63" t="s">
+        <v>187</v>
+      </c>
+      <c r="K63" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J51" t="s">
-        <v>168</v>
-      </c>
-      <c r="K51" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" t="s">
-        <v>48</v>
-      </c>
-      <c r="G54" t="s">
-        <v>172</v>
-      </c>
-      <c r="J54" t="s">
-        <v>173</v>
-      </c>
-      <c r="K54" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J55" t="s">
-        <v>78</v>
-      </c>
-      <c r="K55" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" t="s">
-        <v>1</v>
-      </c>
-      <c r="G58" t="s">
-        <v>149</v>
-      </c>
-      <c r="J58" t="s">
-        <v>168</v>
-      </c>
-      <c r="K58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F59" t="s">
-        <v>165</v>
-      </c>
-      <c r="G59" t="s">
-        <v>166</v>
-      </c>
-      <c r="J59" t="s">
-        <v>78</v>
-      </c>
-      <c r="K59" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J60" t="s">
-        <v>178</v>
-      </c>
-      <c r="K60" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" t="s">
-        <v>1</v>
-      </c>
-      <c r="G63" t="s">
-        <v>149</v>
-      </c>
-      <c r="J63" t="s">
-        <v>182</v>
-      </c>
-      <c r="K63" t="s">
-        <v>183</v>
-      </c>
-    </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F64" t="s">
-        <v>165</v>
-      </c>
-      <c r="G64" t="s">
-        <v>166</v>
-      </c>
-      <c r="J64" t="s">
-        <v>78</v>
-      </c>
       <c r="K64" t="s">
-        <v>119</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A40:E40"/>
+  <mergeCells count="14">
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A2:E2"/>
@@ -1959,6 +2039,11 @@
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A44:E44"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1969,15 +2054,16 @@
     <hyperlink ref="A30" r:id="rId5"/>
     <hyperlink ref="A33" r:id="rId6"/>
     <hyperlink ref="A36" r:id="rId7"/>
-    <hyperlink ref="A40" r:id="rId8"/>
+    <hyperlink ref="A39" r:id="rId8"/>
     <hyperlink ref="A44" r:id="rId9"/>
-    <hyperlink ref="A49" r:id="rId10"/>
-    <hyperlink ref="A54" r:id="rId11"/>
-    <hyperlink ref="A58" r:id="rId12"/>
-    <hyperlink ref="A63" r:id="rId13"/>
+    <hyperlink ref="A48" r:id="rId10"/>
+    <hyperlink ref="A52" r:id="rId11"/>
+    <hyperlink ref="A55" r:id="rId12"/>
+    <hyperlink ref="A59" r:id="rId13"/>
+    <hyperlink ref="A62" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>